<commit_message>
index, welcome and intro page
</commit_message>
<xml_diff>
--- a/docs/layout/Auflistung Inhalte.xlsx
+++ b/docs/layout/Auflistung Inhalte.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="8115" windowHeight="3660"/>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>einzelne Bausteine zur Durchführung des ST</t>
-  </si>
-  <si>
-    <t>Online Bucherstellung</t>
   </si>
   <si>
     <t>PP-Vorlage Buch</t>
@@ -449,12 +446,15 @@
       <t xml:space="preserve"> to get the whole material of the Storytelling Club.  </t>
     </r>
   </si>
+  <si>
+    <t>Online Bucherstellung (layouter)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -605,7 +605,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -618,9 +618,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -658,7 +658,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -692,6 +692,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -726,9 +727,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -901,21 +903,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="61.42578125" customWidth="1"/>
     <col min="3" max="3" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -932,20 +934,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="330.75">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -956,7 +958,7 @@
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
@@ -967,18 +969,18 @@
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>15</v>
       </c>
@@ -989,20 +991,20 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" ht="63">
+    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>123</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
@@ -1013,18 +1015,18 @@
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75">
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75">
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>21</v>
       </c>
@@ -1035,7 +1037,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75">
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
@@ -1046,20 +1048,20 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" ht="94.5">
+    <row r="12" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75">
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
@@ -1070,7 +1072,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75">
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
@@ -1081,502 +1083,502 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75">
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75">
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75">
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75">
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75">
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75">
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75">
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75">
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75">
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75">
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="31.5">
+    <row r="25" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="31.5">
+    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="31.5">
+    <row r="27" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="31.5">
+    <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="31.5">
+    <row r="29" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="31.5">
+    <row r="30" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="31.5">
+    <row r="31" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="31.5">
+    <row r="32" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75">
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75">
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="15.75">
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75">
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75">
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75">
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75">
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75">
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" ht="15.75">
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="15.75">
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75">
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75">
+    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75">
+    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75">
+    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="1:5" ht="15.75">
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75">
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75">
+    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75">
+    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75">
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75">
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75">
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75">
+    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" ht="15.75">
+    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" ht="15.75">
+    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75">
+    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="1:5" ht="15.75">
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5" ht="15.75">
+    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75">
+    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="1"/>
@@ -1588,16 +1590,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1608,12 +1610,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>